<commit_message>
some prep for rerunning the experiments
</commit_message>
<xml_diff>
--- a/calypso_simulation/test_data/concurrent/caly-conc-100.xlsx
+++ b/calypso_simulation/test_data/concurrent/caly-conc-100.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alp/go-workspace/src/github.com/ceyhunalp/calypso_experiments/calypso_simulation/test_data/concurrent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493A4FE-1D11-8742-9CBB-70DD435DCB8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0CF35C-8FEB-C846-9469-B7860657CAE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31400" yWindow="-20" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1232,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S112"/>
+  <dimension ref="A1:W511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="Q103" sqref="Q103:S112"/>
+    <sheetView tabSelected="1" topLeftCell="O492" workbookViewId="0">
+      <selection activeCell="Q505" sqref="Q505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6043,7 +6043,7 @@
         <v>20.825493999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>24.192488000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>23.78914</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>23.798943000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>23.958368</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>21.133417000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>112</v>
       </c>
@@ -6348,8 +6348,9 @@
       <c r="S103" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W103"/>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>108</v>
       </c>
@@ -6426,7 +6427,7 @@
         <v>26.407315768000004</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>109</v>
       </c>
@@ -6503,7 +6504,7 @@
         <v>26.893461899999998</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>110</v>
       </c>
@@ -6580,7 +6581,7 @@
         <v>20.695249</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>111</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>30.786887199999999</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>115</v>
       </c>
@@ -6734,7 +6735,7 @@
         <v>21.298622660000003</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>104</v>
       </c>
@@ -6811,7 +6812,7 @@
         <v>23.798605299999998</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>105</v>
       </c>
@@ -6888,7 +6889,7 @@
         <v>29.6374779</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>106</v>
       </c>
@@ -6965,7 +6966,7 @@
         <v>30.716476590000003</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>107</v>
       </c>
@@ -7041,6 +7042,33 @@
         <f>_xlfn.PERCENTILE.INC(($D112,$G112,$J112,$M112,$P112),0.95)</f>
         <v>30.764514716000001</v>
       </c>
+    </row>
+    <row r="503" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W503" s="2"/>
+    </row>
+    <row r="504" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W504" s="2"/>
+    </row>
+    <row r="505" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W505" s="2"/>
+    </row>
+    <row r="506" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W506" s="2"/>
+    </row>
+    <row r="507" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W507" s="2"/>
+    </row>
+    <row r="508" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W508" s="2"/>
+    </row>
+    <row r="509" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W509" s="2"/>
+    </row>
+    <row r="510" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W510" s="2"/>
+    </row>
+    <row r="511" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="W511" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>